<commit_message>
Atualização do Implementation Guide.
</commit_message>
<xml_diff>
--- a/StructureDefinition-live-alone-pre-stroke-extension.xlsx
+++ b/StructureDefinition-live-alone-pre-stroke-extension.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://www.gabriellesantosleandro.com/molic-avc/StructureDefinition/live-alone-pre-stroke-extension</t>
+    <t>https://molic-avc.gabriellesantosleandro.com/StructureDefinition/live-alone-pre-stroke-extension</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-15T15:21:17-03:00</t>
+    <t>2023-08-16T00:27:03-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -227,7 +227,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>https://www.gabriellesantosleandro.com/molic-avc/ValueSet/live-alone-pre-stroke</t>
+    <t>https://molic-avc.gabriellesantosleandro.com/ValueSet/live-alone-pre-stroke</t>
   </si>
   <si>
     <t xml:space="preserve">ext-1
@@ -570,7 +570,7 @@
     <col min="23" max="23" width="1.0390625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="8.734375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="1.0390625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="75.765625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="70.19921875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.0390625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="9.546875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>

</xml_diff>